<commit_message>
ajout du tableau de synthèse
</commit_message>
<xml_diff>
--- a/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
+++ b/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainpailler/Documents/BTS/Portfolio/portfolio-2023/src/assets/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA218EED-454B-F143-9D73-E45B53531A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB59630-4311-4A49-A013-BAAB0AE633CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -188,6 +188,33 @@
   </si>
   <si>
     <t>N° candidat :  02341329386</t>
+  </si>
+  <si>
+    <t>09/05/2023 au 27/06/2023</t>
+  </si>
+  <si>
+    <t>03/03/2023 au 01/05/2024</t>
+  </si>
+  <si>
+    <t>24/10/2023 au 15/01/2024</t>
+  </si>
+  <si>
+    <t>Développement d'une API (NodeJs)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>07/11/2023 au 15/01/2024</t>
+  </si>
+  <si>
+    <t>Création d'une Base de données (MySql)</t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un outil d'inventaire et ticketing (GLPI)</t>
+  </si>
+  <si>
+    <t>21/11/2022 au 21/11/2022</t>
   </si>
 </sst>
 </file>
@@ -197,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -260,8 +287,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -665,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -730,77 +762,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1110,10 +1148,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1131,56 +1169,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="44" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="45"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1192,22 +1230,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1230,8 +1268,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
@@ -1287,16 +1325,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1342,7 +1380,7 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="45" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="15"/>
@@ -1395,7 +1433,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="45" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="16"/>
@@ -1445,7 +1483,7 @@
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="45" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="15"/>
@@ -1498,7 +1536,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="46" t="s">
         <v>27</v>
       </c>
       <c r="I12"/>
@@ -1544,7 +1582,7 @@
       <c r="B13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="45" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="15"/>
@@ -1600,7 +1638,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="46" t="s">
         <v>27</v>
       </c>
       <c r="I14"/>
@@ -1643,12 +1681,14 @@
       <c r="A15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="45" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="16"/>
@@ -1692,13 +1732,15 @@
       <c r="A16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="46" t="s">
         <v>27</v>
       </c>
       <c r="I16"/>
@@ -1738,13 +1780,23 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>27</v>
+      </c>
       <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="47" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="45" t="s">
+        <v>27</v>
+      </c>
       <c r="H17" s="16"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -1783,13 +1835,25 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>27</v>
+      </c>
       <c r="H18" s="16"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -1827,17 +1891,19 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1874,23 +1940,17 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="16"/>
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A20" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1929,14 +1989,20 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15" t="s">
+      <c r="E21" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="45" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="16"/>
@@ -1978,16 +2044,16 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="15" t="s">
+      <c r="F22" s="15"/>
+      <c r="G22" s="45" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="16"/>
@@ -2028,13 +2094,21 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="F23" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>27</v>
+      </c>
       <c r="H23" s="16"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -2207,17 +2281,15 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2254,15 +2326,17 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A28" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2524,15 +2598,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2569,15 +2643,15 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2614,7 +2688,51 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+    </row>
     <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -2660,20 +2778,21 @@
     <row r="79" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="80" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2684,9 +2803,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2804,19 +2926,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4E27C2-9E50-4B05-A279-A1A1A8E00469}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0BFF56-BE1D-4AD9-9F23-E461DD70F79B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2838,9 +2956,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0BFF56-BE1D-4AD9-9F23-E461DD70F79B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4E27C2-9E50-4B05-A279-A1A1A8E00469}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ajout de la modif du tableau de synthèse
</commit_message>
<xml_diff>
--- a/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
+++ b/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainpailler/Documents/BTS/Portfolio/portfolio-2023/src/assets/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB59630-4311-4A49-A013-BAAB0AE633CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEBF2E4-72F3-7B4B-9F38-171CC5E4F013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>21/11/2022 au 21/11/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1153,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2104,7 +2107,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="45" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="G23" s="47" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
ajout du nouveau cv + tableau de synthèse
</commit_message>
<xml_diff>
--- a/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
+++ b/src/assets/portfolio/Tableau-de-synthese-E4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainpailler/Documents/BTS/Portfolio/portfolio-2023/src/assets/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEBF2E4-72F3-7B4B-9F38-171CC5E4F013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E41E4-ABFA-D441-9427-0B881BD1A6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -132,9 +132,6 @@
     <t>SESSION 2024</t>
   </si>
   <si>
-    <t>10/10/2022 au 06/02/2023</t>
-  </si>
-  <si>
     <t>Centre de formation : IPSSI Formation</t>
   </si>
   <si>
@@ -157,21 +154,9 @@
     <t>Inventaire des équipements réseaux</t>
   </si>
   <si>
-    <t>06/02/2023 au 01/04/2023</t>
-  </si>
-  <si>
-    <t>07/11/2022 au 07/11/2022</t>
-  </si>
-  <si>
-    <t>08/11/2022 au 08/11/2022</t>
-  </si>
-  <si>
     <t>Mettre en place un outil de veille technologique</t>
   </si>
   <si>
-    <t>10/10/2022 au 03/05/2024</t>
-  </si>
-  <si>
     <t>Developpement d'une application web (site e-commerce)</t>
   </si>
   <si>
@@ -190,34 +175,61 @@
     <t>N° candidat :  02341329386</t>
   </si>
   <si>
-    <t>09/05/2023 au 27/06/2023</t>
-  </si>
-  <si>
-    <t>03/03/2023 au 01/05/2024</t>
-  </si>
-  <si>
-    <t>24/10/2023 au 15/01/2024</t>
-  </si>
-  <si>
     <t>Développement d'une API (NodeJs)</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>07/11/2023 au 15/01/2024</t>
-  </si>
-  <si>
     <t>Création d'une Base de données (MySql)</t>
   </si>
   <si>
     <t>Installation et configuration d'un outil d'inventaire et ticketing (GLPI)</t>
   </si>
   <si>
-    <t>21/11/2022 au 21/11/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>10/10/22 au 06/02/23</t>
+  </si>
+  <si>
+    <t>06/02/23 au 01/04/23</t>
+  </si>
+  <si>
+    <t>07/11/22 au 07/11/22</t>
+  </si>
+  <si>
+    <t>08/11/22 au 08/11/22</t>
+  </si>
+  <si>
+    <t>10/10/22 au 03/05/24</t>
+  </si>
+  <si>
+    <t>24/10/23 au 15/01/24</t>
+  </si>
+  <si>
+    <t>03/03/23 au 01/05/24</t>
+  </si>
+  <si>
+    <t>07/11/23 au 15/01/24</t>
+  </si>
+  <si>
+    <t>21/11/22 au 21/11/22</t>
+  </si>
+  <si>
+    <t>09/05/23 au 27/06/23</t>
+  </si>
+  <si>
+    <t>Implémentation d'une API</t>
+  </si>
+  <si>
+    <t>11/12/2023 au 26/01/2024</t>
+  </si>
+  <si>
+    <t>Migration d'un composant AngularJS vers Angular2+</t>
+  </si>
+  <si>
+    <t>13/10/2023 au 01/11/2023</t>
   </si>
 </sst>
 </file>
@@ -765,6 +777,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -830,18 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1153,8 +1165,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1172,56 +1184,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1233,22 +1245,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1271,8 +1283,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
@@ -1328,16 +1340,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1376,15 +1388,15 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="45" t="s">
-        <v>27</v>
+      <c r="E9" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -1427,17 +1439,17 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="45" t="s">
-        <v>27</v>
+      <c r="G10" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10"/>
@@ -1478,16 +1490,16 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="45" t="s">
-        <v>27</v>
+      <c r="F11" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="16"/>
@@ -1529,18 +1541,18 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="46" t="s">
-        <v>27</v>
+      <c r="H12" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1580,13 +1592,13 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>27</v>
+        <v>47</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -1631,18 +1643,18 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="46" t="s">
-        <v>27</v>
+      <c r="H14" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1682,17 +1694,17 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="45" t="s">
-        <v>27</v>
+      <c r="G15" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15"/>
@@ -1733,18 +1745,18 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="46" t="s">
-        <v>27</v>
+      <c r="H16" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -1784,21 +1796,21 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>27</v>
+        <v>51</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="15"/>
-      <c r="E17" s="47" t="s">
-        <v>48</v>
+      <c r="E17" s="25" t="s">
+        <v>40</v>
       </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="45" t="s">
-        <v>27</v>
+      <c r="G17" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17"/>
@@ -1839,23 +1851,23 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>27</v>
+      <c r="C18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18"/>
@@ -1896,11 +1908,11 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="45" t="s">
-        <v>27</v>
+      <c r="C19" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -1944,16 +1956,16 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1992,21 +2004,21 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>27</v>
+      <c r="E21" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21"/>
@@ -2047,17 +2059,17 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="45" t="s">
-        <v>27</v>
+      <c r="G22" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22"/>
@@ -2098,19 +2110,19 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>27</v>
+      <c r="F23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23"/>
@@ -2330,16 +2342,16 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2377,13 +2389,21 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="F29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="H29" s="16"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -2422,13 +2442,21 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="F30" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="H30" s="16"/>
       <c r="I30"/>
       <c r="J30"/>
@@ -2806,6 +2834,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2814,7 +2848,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD1390579AA2DB42B60BD32A8BA9EE87" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="117d90f33f91db31950e32585cc871ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b3613ba4871b6d4221e6a6d8c4f7bd5">
     <xsd:element name="properties">
@@ -2928,13 +2962,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4E27C2-9E50-4B05-A279-A1A1A8E00469}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0BFF56-BE1D-4AD9-9F23-E461DD70F79B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2942,7 +2979,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED8E7EB-6AE0-4E06-B60E-AF63C56B7187}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2956,13 +2993,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4E27C2-9E50-4B05-A279-A1A1A8E00469}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>